<commit_message>
align fix for db normalisation
</commit_message>
<xml_diff>
--- a/db_normalisation_build/normalisation_activity_db.xlsx
+++ b/db_normalisation_build/normalisation_activity_db.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" state="visible" r:id="rId2"/>
@@ -195,231 +195,16 @@
     <t xml:space="preserve">Exam Board ID</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1001, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">3, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">4, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">3, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">5</t>
-    </r>
+    <t xml:space="preserve">1001, 1002, 1003, 1004, 1005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1001, 1003, 1004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1002, 1004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1002, 1005</t>
   </si>
 </sst>
 </file>
@@ -430,7 +215,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -460,12 +245,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -510,49 +289,53 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -575,7 +358,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V21" activeCellId="1" sqref="A2:I46 V21"/>
+      <selection pane="topLeft" activeCell="V21" activeCellId="1" sqref="I23:J37 V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -952,20 +735,20 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I44" activeCellId="0" sqref="A2:I46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I44" activeCellId="1" sqref="I23:J37 I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="8.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="9.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="7.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="10.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,13 +799,13 @@
       <c r="F2" s="4" t="n">
         <v>37128</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1033,9 +816,9 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -1044,9 +827,9 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -1067,13 +850,13 @@
       <c r="F5" s="4" t="n">
         <v>37128</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1084,9 +867,9 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
@@ -1095,9 +878,9 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -1118,13 +901,13 @@
       <c r="F8" s="4" t="n">
         <v>37128</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1135,9 +918,9 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -1146,9 +929,9 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
@@ -1169,13 +952,13 @@
       <c r="F11" s="4" t="n">
         <v>36435</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1186,9 +969,9 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
@@ -1197,9 +980,9 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
@@ -1220,13 +1003,13 @@
       <c r="F14" s="4" t="n">
         <v>36435</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1237,9 +1020,9 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
@@ -1248,9 +1031,9 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
@@ -1271,13 +1054,13 @@
       <c r="F17" s="4" t="n">
         <v>36435</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1288,9 +1071,9 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
@@ -1299,9 +1082,9 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
@@ -1322,13 +1105,13 @@
       <c r="F20" s="4" t="n">
         <v>34855</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1339,9 +1122,9 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
@@ -1350,9 +1133,9 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
@@ -1373,13 +1156,13 @@
       <c r="F23" s="4" t="n">
         <v>34855</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1390,9 +1173,9 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
@@ -1401,9 +1184,9 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
@@ -1424,13 +1207,13 @@
       <c r="F26" s="4" t="n">
         <v>34855</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1441,9 +1224,9 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
@@ -1452,9 +1235,9 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="n">
@@ -1475,13 +1258,13 @@
       <c r="F29" s="4" t="n">
         <v>29436</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1492,9 +1275,9 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
@@ -1503,9 +1286,9 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="n">
@@ -1526,13 +1309,13 @@
       <c r="F32" s="4" t="n">
         <v>29436</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1543,9 +1326,9 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
@@ -1554,9 +1337,9 @@
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="n">
@@ -1577,13 +1360,13 @@
       <c r="F35" s="4" t="n">
         <v>29436</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G35" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1594,9 +1377,9 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
@@ -1605,9 +1388,9 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="n">
@@ -1628,13 +1411,13 @@
       <c r="F38" s="4" t="n">
         <v>37377</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H38" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="I38" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1645,9 +1428,9 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
@@ -1656,9 +1439,9 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="n">
@@ -1679,13 +1462,13 @@
       <c r="F41" s="4" t="n">
         <v>37377</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H41" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I41" s="6" t="s">
+      <c r="I41" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1696,9 +1479,9 @@
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
@@ -1707,9 +1490,9 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="n">
@@ -1730,13 +1513,13 @@
       <c r="F44" s="4" t="n">
         <v>37377</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="G44" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="H44" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I44" s="6" t="s">
+      <c r="I44" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1747,9 +1530,9 @@
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
@@ -1758,9 +1541,9 @@
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="135">
@@ -1917,20 +1700,20 @@
   </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="A2:I46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="I23:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="26.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="27.26"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,7 +1735,7 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1975,7 +1758,7 @@
       <c r="F2" s="4" t="n">
         <v>37128</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1986,7 +1769,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="9"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -1995,7 +1778,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="9"/>
+      <c r="G4" s="10"/>
       <c r="I4" s="2" t="s">
         <v>46</v>
       </c>
@@ -2028,19 +1811,19 @@
       <c r="F5" s="4" t="n">
         <v>36435</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="6" t="n">
+      <c r="K5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2051,11 +1834,11 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="9"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="G6" s="10"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
@@ -2064,11 +1847,11 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="9"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="G7" s="10"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -2089,19 +1872,19 @@
       <c r="F8" s="4" t="n">
         <v>34855</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="6" t="n">
+      <c r="K8" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2112,11 +1895,11 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="9"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="G9" s="10"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -2125,11 +1908,11 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="9"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="G10" s="10"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
@@ -2150,19 +1933,19 @@
       <c r="F11" s="4" t="n">
         <v>29436</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="6" t="n">
+      <c r="I11" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="6" t="n">
+      <c r="K11" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="L11" s="6" t="n">
+      <c r="L11" s="8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2173,11 +1956,11 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="9"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="G12" s="10"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
@@ -2186,11 +1969,11 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="9"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="G13" s="10"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
@@ -2211,19 +1994,19 @@
       <c r="F14" s="4" t="n">
         <v>37377</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="6" t="n">
+      <c r="I14" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="6" t="n">
+      <c r="K14" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="L14" s="5" t="n">
+      <c r="L14" s="7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2234,11 +2017,11 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="9"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="G15" s="10"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
@@ -2247,34 +2030,34 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="9"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="G16" s="10"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I17" s="6" t="n">
+      <c r="I17" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K17" s="6" t="n">
+      <c r="K17" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="L17" s="6" t="n">
+      <c r="L17" s="8" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -2283,39 +2066,39 @@
       <c r="E19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C20" s="6" t="n">
+      <c r="C20" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="6" t="n">
+      <c r="E20" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="9"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="10"/>
       <c r="I22" s="2" t="s">
         <v>56</v>
       </c>
@@ -2324,164 +2107,164 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C23" s="6" t="n">
+      <c r="C23" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="6" t="n">
+      <c r="E23" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="1" t="n">
+      <c r="I23" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="6" t="n">
+      <c r="C26" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="6" t="n">
+      <c r="E26" s="8" t="n">
         <v>3</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="I26" s="1" t="n">
+      <c r="I26" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
       <c r="F27" s="10"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
       <c r="F28" s="10"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="6" t="n">
+      <c r="C29" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="6" t="n">
+      <c r="E29" s="8" t="n">
         <v>4</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="1" t="n">
+      <c r="I29" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
       <c r="F30" s="10"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="10"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C32" s="6" t="n">
+      <c r="C32" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="6" t="n">
+      <c r="E32" s="8" t="n">
         <v>5</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="I32" s="1" t="n">
+      <c r="I32" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J32" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
       <c r="F33" s="10"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
       <c r="F34" s="10"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I35" s="1" t="n">
+      <c r="I35" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="J35" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="85">

</xml_diff>